<commit_message>
Terminada parte de gramatica falta manejar errores
</commit_message>
<xml_diff>
--- a/Documentacion/Tabla de analisis sintactico-Proyecto 2.xlsx
+++ b/Documentacion/Tabla de analisis sintactico-Proyecto 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalej\Documents\Universidad\Lenguajes formales y de programacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalej\Documents\C# Projects\Analizador Lexico\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43553089-6B86-42DF-B608-D9CF1DEF5F1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D51A0C5-0C85-4985-84CB-892AA1D8A89D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{8FA35D13-EE7F-4D24-ABCB-73E245BD8EA5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="141">
   <si>
     <t>A</t>
   </si>
@@ -306,9 +306,6 @@
     <t>DESDE ID = ENTERO HASTA ID S’’ ENTERO INCREMENTO ENTERO S’</t>
   </si>
   <si>
-    <t>(V’ X V’) Q’</t>
-  </si>
-  <si>
     <t>V’ X V’</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t xml:space="preserve">|| V </t>
   </si>
   <si>
-    <t>{L}</t>
-  </si>
-  <si>
     <t>SINO_SI(V) S’ E</t>
   </si>
   <si>
@@ -445,6 +439,15 @@
   </si>
   <si>
     <t>= Q''</t>
+  </si>
+  <si>
+    <t>Q'''</t>
+  </si>
+  <si>
+    <t>(V’ X V’) Q'''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{L} </t>
   </si>
 </sst>
 </file>
@@ -944,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF91B6D2-3D05-4DAC-9F15-996E1E4A83AD}">
   <dimension ref="B2:AU36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" topLeftCell="AD7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AH32" sqref="AH32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,6 +964,7 @@
     <col min="15" max="15" width="24.42578125" customWidth="1"/>
     <col min="16" max="16" width="64.140625" customWidth="1"/>
     <col min="18" max="18" width="15.140625" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
     <col min="22" max="22" width="13.140625" customWidth="1"/>
     <col min="23" max="23" width="11.5703125" customWidth="1"/>
     <col min="24" max="24" width="13.28515625" customWidth="1"/>
@@ -971,7 +975,7 @@
   <sheetData>
     <row r="2" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -1025,7 +1029,7 @@
         <v>40</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U2" t="s">
         <v>42</v>
@@ -1034,10 +1038,10 @@
         <v>43</v>
       </c>
       <c r="W2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="X2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Y2" t="s">
         <v>46</v>
@@ -1046,22 +1050,22 @@
         <v>16</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AC2" t="s">
         <v>47</v>
       </c>
       <c r="AD2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF2" t="s">
         <v>108</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>110</v>
       </c>
       <c r="AG2" t="s">
         <v>48</v>
@@ -1106,7 +1110,7 @@
         <v>63</v>
       </c>
       <c r="AU2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:47" x14ac:dyDescent="0.25">
@@ -1210,22 +1214,22 @@
         <v>3</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="S7" s="2"/>
       <c r="Y7" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:47" x14ac:dyDescent="0.25">
@@ -1233,59 +1237,59 @@
         <v>4</v>
       </c>
       <c r="S8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V8" t="s">
         <v>43</v>
       </c>
       <c r="W8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="X8" t="s">
         <v>45</v>
       </c>
       <c r="AG8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="S9" t="s">
+        <v>105</v>
+      </c>
+      <c r="T9" t="s">
+        <v>103</v>
+      </c>
+      <c r="U9" t="s">
         <v>104</v>
       </c>
-      <c r="S9" t="s">
-        <v>107</v>
-      </c>
-      <c r="T9" t="s">
-        <v>105</v>
-      </c>
-      <c r="U9" t="s">
-        <v>106</v>
-      </c>
       <c r="AG9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AC10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AF10" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="AE10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF10" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="AH10" t="s">
         <v>62</v>
@@ -1296,10 +1300,10 @@
     </row>
     <row r="11" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
@@ -1310,13 +1314,13 @@
     </row>
     <row r="12" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="S12" t="s">
+        <v>126</v>
+      </c>
+      <c r="W12" t="s">
         <v>125</v>
-      </c>
-      <c r="S12" t="s">
-        <v>128</v>
-      </c>
-      <c r="W12" t="s">
-        <v>127</v>
       </c>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
@@ -1368,7 +1372,7 @@
         <v>7</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Z15" t="s">
         <v>78</v>
@@ -1382,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="Z16" t="s">
         <v>78</v>
@@ -1397,16 +1401,16 @@
       </c>
       <c r="Y17" s="1"/>
       <c r="AC17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE17" t="s">
         <v>130</v>
       </c>
-      <c r="AD17" s="1" t="s">
+      <c r="AF17" t="s">
         <v>131</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>133</v>
       </c>
       <c r="AH17" t="s">
         <v>62</v>
@@ -1417,17 +1421,17 @@
     </row>
     <row r="18" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="S18" t="s">
+        <v>133</v>
+      </c>
+      <c r="U18" t="s">
         <v>134</v>
-      </c>
-      <c r="S18" t="s">
-        <v>135</v>
-      </c>
-      <c r="U18" t="s">
-        <v>136</v>
       </c>
       <c r="Y18" s="1"/>
       <c r="AG18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="2:46" x14ac:dyDescent="0.25">
@@ -1449,7 +1453,7 @@
         <v>10</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Z20" t="s">
         <v>78</v>
@@ -1463,7 +1467,7 @@
         <v>11</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Z21" t="s">
         <v>78</v>
@@ -1575,22 +1579,22 @@
         <v>20</v>
       </c>
       <c r="S29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AG29" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="2:46" x14ac:dyDescent="0.25">
@@ -1638,13 +1642,16 @@
     </row>
     <row r="32" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>23</v>
+        <v>138</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>62</v>
       </c>
       <c r="AO32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP32" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="AP32" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33" spans="2:43" x14ac:dyDescent="0.25">
@@ -1652,7 +1659,7 @@
         <v>24</v>
       </c>
       <c r="AQ33" s="2" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="2:43" x14ac:dyDescent="0.25">
@@ -1704,7 +1711,7 @@
         <v>62</v>
       </c>
       <c r="L35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M35" t="s">
         <v>62</v>
@@ -1751,7 +1758,7 @@
         <v>62</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N36" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Controla errores en declaracion de variables
</commit_message>
<xml_diff>
--- a/Documentacion/Tabla de analisis sintactico-Proyecto 2.xlsx
+++ b/Documentacion/Tabla de analisis sintactico-Proyecto 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalej\Documents\C# Projects\Analizador Lexico\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D51A0C5-0C85-4985-84CB-892AA1D8A89D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FBB1C0-6CDD-48BA-B7F7-56D619703981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{8FA35D13-EE7F-4D24-ABCB-73E245BD8EA5}"/>
   </bookViews>
@@ -429,9 +429,6 @@
     <t>ID Q'</t>
   </si>
   <si>
-    <t>DECIMAL Q'</t>
-  </si>
-  <si>
     <t>(Q'')Q'</t>
   </si>
   <si>
@@ -448,6 +445,9 @@
   </si>
   <si>
     <t xml:space="preserve">{L} </t>
+  </si>
+  <si>
+    <t>ENTERO Q'</t>
   </si>
 </sst>
 </file>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF91B6D2-3D05-4DAC-9F15-996E1E4A83AD}">
   <dimension ref="B2:AU36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH32" sqref="AH32"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1372,7 @@
         <v>7</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Z15" t="s">
         <v>78</v>
@@ -1386,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z16" t="s">
         <v>78</v>
@@ -1426,12 +1426,12 @@
       <c r="S18" t="s">
         <v>133</v>
       </c>
-      <c r="U18" t="s">
-        <v>134</v>
+      <c r="T18" t="s">
+        <v>140</v>
       </c>
       <c r="Y18" s="1"/>
       <c r="AG18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="2:46" x14ac:dyDescent="0.25">
@@ -1594,7 +1594,7 @@
         <v>93</v>
       </c>
       <c r="AG29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="2:46" x14ac:dyDescent="0.25">
@@ -1642,7 +1642,7 @@
     </row>
     <row r="32" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AH32" t="s">
         <v>62</v>
@@ -1659,7 +1659,7 @@
         <v>24</v>
       </c>
       <c r="AQ33" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="2:43" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Trabajando en tabla de simbolos
</commit_message>
<xml_diff>
--- a/Documentacion/Tabla de analisis sintactico-Proyecto 2.xlsx
+++ b/Documentacion/Tabla de analisis sintactico-Proyecto 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalej\Documents\C# Projects\Analizador Lexico\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FBB1C0-6CDD-48BA-B7F7-56D619703981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E319A602-E591-425B-9C26-0CF08A01EB57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{8FA35D13-EE7F-4D24-ABCB-73E245BD8EA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8FA35D13-EE7F-4D24-ABCB-73E245BD8EA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF91B6D2-3D05-4DAC-9F15-996E1E4A83AD}">
   <dimension ref="B2:AU36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>